<commit_message>
Settings save button fixed
</commit_message>
<xml_diff>
--- a/data/locations/BC.xlsx
+++ b/data/locations/BC.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Cableway BC" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Weir BC" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9424" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9627" uniqueCount="948">
   <si>
     <t>General Information</t>
   </si>
@@ -2552,6 +2553,309 @@
   </si>
   <si>
     <t>-128.32466</t>
+  </si>
+  <si>
+    <t>08NE087</t>
+  </si>
+  <si>
+    <t>Weir</t>
+  </si>
+  <si>
+    <t>DEER CREEK AT DEER PARK</t>
+  </si>
+  <si>
+    <t>49.44847</t>
+  </si>
+  <si>
+    <t>-118.042</t>
+  </si>
+  <si>
+    <t>08NH115</t>
+  </si>
+  <si>
+    <t>SULLIVAN CREEK NEAR CANYON</t>
+  </si>
+  <si>
+    <t>49.10427</t>
+  </si>
+  <si>
+    <t>-116.43675</t>
+  </si>
+  <si>
+    <t>08NJ130</t>
+  </si>
+  <si>
+    <t>ANDERSON CREEK NEAR NELSON</t>
+  </si>
+  <si>
+    <t>49.50195</t>
+  </si>
+  <si>
+    <t>-117.26128</t>
+  </si>
+  <si>
+    <t>08HA016</t>
+  </si>
+  <si>
+    <t>BINGS CREEK NEAR THE MOUTH</t>
+  </si>
+  <si>
+    <t>48.78922</t>
+  </si>
+  <si>
+    <t>-123.72547</t>
+  </si>
+  <si>
+    <t>08GA061</t>
+  </si>
+  <si>
+    <t>MACKAY CREEK AT MONTROYAL BOULEVARD</t>
+  </si>
+  <si>
+    <t>49.35616</t>
+  </si>
+  <si>
+    <t>-123.09986</t>
+  </si>
+  <si>
+    <t>08MH152</t>
+  </si>
+  <si>
+    <t>BERTRAND CREEK AT INTERNATIONAL BOUNDARY</t>
+  </si>
+  <si>
+    <t>49.00239</t>
+  </si>
+  <si>
+    <t>-122.5234</t>
+  </si>
+  <si>
+    <t>08OA003</t>
+  </si>
+  <si>
+    <t>PREMIER CREEK NEAR DAAJING GIIDS</t>
+  </si>
+  <si>
+    <t>53.25861</t>
+  </si>
+  <si>
+    <t>-132.07505</t>
+  </si>
+  <si>
+    <t>08EE025</t>
+  </si>
+  <si>
+    <t>TWO MILE CREEK IN DISTRICT LOT 4834</t>
+  </si>
+  <si>
+    <t>55.29611</t>
+  </si>
+  <si>
+    <t>-127.62075</t>
+  </si>
+  <si>
+    <t>08JB013</t>
+  </si>
+  <si>
+    <t>NORTH BEACH CREEK ABOVE ALLIN CREEK</t>
+  </si>
+  <si>
+    <t>54.12694</t>
+  </si>
+  <si>
+    <t>-125.92833</t>
+  </si>
+  <si>
+    <t>08LB024</t>
+  </si>
+  <si>
+    <t>FISHTRAP CREEK NEAR MCLURE</t>
+  </si>
+  <si>
+    <t>51.12203</t>
+  </si>
+  <si>
+    <t>-120.20894</t>
+  </si>
+  <si>
+    <t>08LE108</t>
+  </si>
+  <si>
+    <t>EAST CANOE CREEK ABOVE DAM</t>
+  </si>
+  <si>
+    <t>50.69665</t>
+  </si>
+  <si>
+    <t>-119.19616</t>
+  </si>
+  <si>
+    <t>08LF007</t>
+  </si>
+  <si>
+    <t>CRISS CREEK NEAR SAVONA</t>
+  </si>
+  <si>
+    <t>50.8839</t>
+  </si>
+  <si>
+    <t>-120.96594</t>
+  </si>
+  <si>
+    <t>08LG056</t>
+  </si>
+  <si>
+    <t>GUICHON CREEK ABOVE TUNKWA LAKE DIVERSION</t>
+  </si>
+  <si>
+    <t>50.60783</t>
+  </si>
+  <si>
+    <t>-120.91086</t>
+  </si>
+  <si>
+    <t>08NM065</t>
+  </si>
+  <si>
+    <t>VERNON CREEK AT OUTLET OF KALAMALKA LAKE</t>
+  </si>
+  <si>
+    <t>50.23847</t>
+  </si>
+  <si>
+    <t>-119.26689</t>
+  </si>
+  <si>
+    <t>08NM134</t>
+  </si>
+  <si>
+    <t>CAMP CREEK AT MOUTH NEAR THIRSK</t>
+  </si>
+  <si>
+    <t>49.71234</t>
+  </si>
+  <si>
+    <t>-120.01117</t>
+  </si>
+  <si>
+    <t>08NM139</t>
+  </si>
+  <si>
+    <t>ESPERON CREEK NEAR KELOWNA</t>
+  </si>
+  <si>
+    <t>50.07333</t>
+  </si>
+  <si>
+    <t>-119.68778</t>
+  </si>
+  <si>
+    <t>08NM146</t>
+  </si>
+  <si>
+    <t>CLARK CREEK NEAR WINFIELD</t>
+  </si>
+  <si>
+    <t>50.04875</t>
+  </si>
+  <si>
+    <t>-119.33597</t>
+  </si>
+  <si>
+    <t>08NM165</t>
+  </si>
+  <si>
+    <t>LAMBLY CREEK ABOVE TERRACE CREEK</t>
+  </si>
+  <si>
+    <t>49.99417</t>
+  </si>
+  <si>
+    <t>-119.61444</t>
+  </si>
+  <si>
+    <t>08NM172</t>
+  </si>
+  <si>
+    <t>PEARSON CREEK NEAR THE MOUTH</t>
+  </si>
+  <si>
+    <t>49.88694</t>
+  </si>
+  <si>
+    <t>-119.06167</t>
+  </si>
+  <si>
+    <t>08NM173</t>
+  </si>
+  <si>
+    <t>GREATA CREEK NEAR THE MOUTH</t>
+  </si>
+  <si>
+    <t>49.79458</t>
+  </si>
+  <si>
+    <t>-119.85203</t>
+  </si>
+  <si>
+    <t>08NM240</t>
+  </si>
+  <si>
+    <t>TWO FORTY CREEK NEAR PENTICTON</t>
+  </si>
+  <si>
+    <t>49.65089</t>
+  </si>
+  <si>
+    <t>-119.40003</t>
+  </si>
+  <si>
+    <t>08NM241</t>
+  </si>
+  <si>
+    <t>TWO FORTY-ONE CREEK NEAR PENTICTON</t>
+  </si>
+  <si>
+    <t>49.65004</t>
+  </si>
+  <si>
+    <t>-119.39385</t>
+  </si>
+  <si>
+    <t>08NM242</t>
+  </si>
+  <si>
+    <t>DENNIS CREEK NEAR 1780 METRE CONTOUR</t>
+  </si>
+  <si>
+    <t>49.62417</t>
+  </si>
+  <si>
+    <t>-119.38143</t>
+  </si>
+  <si>
+    <t>07SB003</t>
+  </si>
+  <si>
+    <t>YELLOWKNIFE RIVER AT INLET TO PROSPEROUS LAKE</t>
+  </si>
+  <si>
+    <t>62.672</t>
+  </si>
+  <si>
+    <t>-114.26122</t>
+  </si>
+  <si>
+    <t>07SB012</t>
+  </si>
+  <si>
+    <t>DUNCAN LAKE NEAR YELLOWKNIFE</t>
+  </si>
+  <si>
+    <t>62.80781</t>
+  </si>
+  <si>
+    <t>-114.03336</t>
   </si>
 </sst>
 </file>
@@ -31511,4 +31815,682 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>847</v>
+      </c>
+      <c r="B3" t="s">
+        <v>848</v>
+      </c>
+      <c r="C3" t="s">
+        <v>849</v>
+      </c>
+      <c r="D3" t="s">
+        <v>850</v>
+      </c>
+      <c r="E3" t="s">
+        <v>851</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>852</v>
+      </c>
+      <c r="B4" t="s">
+        <v>848</v>
+      </c>
+      <c r="C4" t="s">
+        <v>853</v>
+      </c>
+      <c r="D4" t="s">
+        <v>854</v>
+      </c>
+      <c r="E4" t="s">
+        <v>855</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>856</v>
+      </c>
+      <c r="B5" t="s">
+        <v>848</v>
+      </c>
+      <c r="C5" t="s">
+        <v>857</v>
+      </c>
+      <c r="D5" t="s">
+        <v>858</v>
+      </c>
+      <c r="E5" t="s">
+        <v>859</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>860</v>
+      </c>
+      <c r="B6" t="s">
+        <v>848</v>
+      </c>
+      <c r="C6" t="s">
+        <v>861</v>
+      </c>
+      <c r="D6" t="s">
+        <v>862</v>
+      </c>
+      <c r="E6" t="s">
+        <v>863</v>
+      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>848</v>
+      </c>
+      <c r="C7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>864</v>
+      </c>
+      <c r="B8" t="s">
+        <v>848</v>
+      </c>
+      <c r="C8" t="s">
+        <v>865</v>
+      </c>
+      <c r="D8" t="s">
+        <v>866</v>
+      </c>
+      <c r="E8" t="s">
+        <v>867</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>868</v>
+      </c>
+      <c r="B9" t="s">
+        <v>848</v>
+      </c>
+      <c r="C9" t="s">
+        <v>869</v>
+      </c>
+      <c r="D9" t="s">
+        <v>870</v>
+      </c>
+      <c r="E9" t="s">
+        <v>871</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>872</v>
+      </c>
+      <c r="B10" t="s">
+        <v>848</v>
+      </c>
+      <c r="C10" t="s">
+        <v>873</v>
+      </c>
+      <c r="D10" t="s">
+        <v>874</v>
+      </c>
+      <c r="E10" t="s">
+        <v>875</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>876</v>
+      </c>
+      <c r="B11" t="s">
+        <v>848</v>
+      </c>
+      <c r="C11" t="s">
+        <v>877</v>
+      </c>
+      <c r="D11" t="s">
+        <v>878</v>
+      </c>
+      <c r="E11" t="s">
+        <v>879</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>880</v>
+      </c>
+      <c r="B12" t="s">
+        <v>848</v>
+      </c>
+      <c r="C12" t="s">
+        <v>881</v>
+      </c>
+      <c r="D12" t="s">
+        <v>882</v>
+      </c>
+      <c r="E12" t="s">
+        <v>883</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>884</v>
+      </c>
+      <c r="B13" t="s">
+        <v>848</v>
+      </c>
+      <c r="C13" t="s">
+        <v>885</v>
+      </c>
+      <c r="D13" t="s">
+        <v>886</v>
+      </c>
+      <c r="E13" t="s">
+        <v>887</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>888</v>
+      </c>
+      <c r="B14" t="s">
+        <v>848</v>
+      </c>
+      <c r="C14" t="s">
+        <v>889</v>
+      </c>
+      <c r="D14" t="s">
+        <v>890</v>
+      </c>
+      <c r="E14" t="s">
+        <v>891</v>
+      </c>
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>892</v>
+      </c>
+      <c r="B15" t="s">
+        <v>848</v>
+      </c>
+      <c r="C15" t="s">
+        <v>893</v>
+      </c>
+      <c r="D15" t="s">
+        <v>894</v>
+      </c>
+      <c r="E15" t="s">
+        <v>895</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>896</v>
+      </c>
+      <c r="B16" t="s">
+        <v>848</v>
+      </c>
+      <c r="C16" t="s">
+        <v>897</v>
+      </c>
+      <c r="D16" t="s">
+        <v>898</v>
+      </c>
+      <c r="E16" t="s">
+        <v>899</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>900</v>
+      </c>
+      <c r="B17" t="s">
+        <v>848</v>
+      </c>
+      <c r="C17" t="s">
+        <v>901</v>
+      </c>
+      <c r="D17" t="s">
+        <v>902</v>
+      </c>
+      <c r="E17" t="s">
+        <v>903</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>904</v>
+      </c>
+      <c r="B18" t="s">
+        <v>848</v>
+      </c>
+      <c r="C18" t="s">
+        <v>905</v>
+      </c>
+      <c r="D18" t="s">
+        <v>906</v>
+      </c>
+      <c r="E18" t="s">
+        <v>907</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>908</v>
+      </c>
+      <c r="B19" t="s">
+        <v>848</v>
+      </c>
+      <c r="C19" t="s">
+        <v>909</v>
+      </c>
+      <c r="D19" t="s">
+        <v>910</v>
+      </c>
+      <c r="E19" t="s">
+        <v>911</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>912</v>
+      </c>
+      <c r="B20" t="s">
+        <v>848</v>
+      </c>
+      <c r="C20" t="s">
+        <v>913</v>
+      </c>
+      <c r="D20" t="s">
+        <v>914</v>
+      </c>
+      <c r="E20" t="s">
+        <v>915</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>916</v>
+      </c>
+      <c r="B21" t="s">
+        <v>848</v>
+      </c>
+      <c r="C21" t="s">
+        <v>917</v>
+      </c>
+      <c r="D21" t="s">
+        <v>918</v>
+      </c>
+      <c r="E21" t="s">
+        <v>919</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>819</v>
+      </c>
+      <c r="B22" t="s">
+        <v>848</v>
+      </c>
+      <c r="C22" t="s">
+        <v>820</v>
+      </c>
+      <c r="D22" t="s">
+        <v>821</v>
+      </c>
+      <c r="E22" t="s">
+        <v>822</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>920</v>
+      </c>
+      <c r="B23" t="s">
+        <v>848</v>
+      </c>
+      <c r="C23" t="s">
+        <v>921</v>
+      </c>
+      <c r="D23" t="s">
+        <v>922</v>
+      </c>
+      <c r="E23" t="s">
+        <v>923</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>924</v>
+      </c>
+      <c r="B24" t="s">
+        <v>848</v>
+      </c>
+      <c r="C24" t="s">
+        <v>925</v>
+      </c>
+      <c r="D24" t="s">
+        <v>926</v>
+      </c>
+      <c r="E24" t="s">
+        <v>927</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>928</v>
+      </c>
+      <c r="B25" t="s">
+        <v>848</v>
+      </c>
+      <c r="C25" t="s">
+        <v>929</v>
+      </c>
+      <c r="D25" t="s">
+        <v>930</v>
+      </c>
+      <c r="E25" t="s">
+        <v>931</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>932</v>
+      </c>
+      <c r="B26" t="s">
+        <v>848</v>
+      </c>
+      <c r="C26" t="s">
+        <v>933</v>
+      </c>
+      <c r="D26" t="s">
+        <v>934</v>
+      </c>
+      <c r="E26" t="s">
+        <v>935</v>
+      </c>
+      <c r="F26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>936</v>
+      </c>
+      <c r="B27" t="s">
+        <v>848</v>
+      </c>
+      <c r="C27" t="s">
+        <v>937</v>
+      </c>
+      <c r="D27" t="s">
+        <v>938</v>
+      </c>
+      <c r="E27" t="s">
+        <v>939</v>
+      </c>
+      <c r="F27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>940</v>
+      </c>
+      <c r="B28" t="s">
+        <v>848</v>
+      </c>
+      <c r="C28" t="s">
+        <v>941</v>
+      </c>
+      <c r="D28" t="s">
+        <v>942</v>
+      </c>
+      <c r="E28" t="s">
+        <v>943</v>
+      </c>
+      <c r="F28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>944</v>
+      </c>
+      <c r="B29" t="s">
+        <v>848</v>
+      </c>
+      <c r="C29" t="s">
+        <v>945</v>
+      </c>
+      <c r="D29" t="s">
+        <v>946</v>
+      </c>
+      <c r="E29" t="s">
+        <v>947</v>
+      </c>
+      <c r="F29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>